<commit_message>
Updated pick and place file with correct top/bottom markings as well as assembly zip update.
</commit_message>
<xml_diff>
--- a/Kicad-Faraday/OutputFiles/Faraday-all.xlsx
+++ b/Kicad-Faraday/OutputFiles/Faraday-all.xlsx
@@ -27,9 +27,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>F.Cu</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -357,9 +354,6 @@
     <t>P2</t>
   </si>
   <si>
-    <t>B.Cu</t>
-  </si>
-  <si>
     <t>RefDes</t>
   </si>
   <si>
@@ -472,6 +466,12 @@
   </si>
   <si>
     <t>ST3215SB32768H5HPWAA</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Bottom</t>
   </si>
 </sst>
 </file>
@@ -1317,30 +1317,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" t="s">
         <v>113</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" t="s">
-        <v>115</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -1354,18 +1354,18 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E2">
         <v>270</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1.7549999999999999</v>
@@ -1374,18 +1374,18 @@
         <v>0.51</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E3">
         <v>270</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>2.16</v>
@@ -1394,18 +1394,18 @@
         <v>0.875</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2.12</v>
@@ -1414,18 +1414,18 @@
         <v>0.82</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>1.8</v>
@@ -1434,18 +1434,18 @@
         <v>1.03</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E6">
         <v>90</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>1.855</v>
@@ -1454,18 +1454,18 @@
         <v>1.02</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E7">
         <v>90</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1.83</v>
@@ -1474,18 +1474,18 @@
         <v>0.39</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E8">
         <v>90</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1.62</v>
@@ -1494,18 +1494,18 @@
         <v>0.39</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E9">
         <v>90</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>1.5649999999999999</v>
@@ -1514,18 +1514,18 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E10">
         <v>180</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>0.59</v>
@@ -1534,18 +1534,18 @@
         <v>1.26</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>1.5349999999999999</v>
@@ -1554,18 +1554,18 @@
         <v>0.91</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>1.85</v>
@@ -1574,18 +1574,18 @@
         <v>0.505</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E13">
         <v>270</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>1.5</v>
@@ -1594,18 +1594,18 @@
         <v>0.61</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E14">
         <v>180</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>1.575</v>
@@ -1614,18 +1614,18 @@
         <v>0.59499999999999997</v>
       </c>
       <c r="D15" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E15">
         <v>270</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>0.16</v>
@@ -1634,18 +1634,18 @@
         <v>0.23</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>1.5</v>
@@ -1654,18 +1654,18 @@
         <v>0.52</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E17">
         <v>180</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>2.5</v>
@@ -1674,18 +1674,18 @@
         <v>1.605</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E18">
         <v>90</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>1.5</v>
@@ -1694,18 +1694,18 @@
         <v>0.56499999999999995</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E19">
         <v>180</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>2.355</v>
@@ -1714,18 +1714,18 @@
         <v>1.605</v>
       </c>
       <c r="D20" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E20">
         <v>90</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>1.405</v>
@@ -1734,18 +1734,18 @@
         <v>0.47499999999999998</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>0.61</v>
@@ -1754,18 +1754,18 @@
         <v>1.18</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>0.8</v>
@@ -1774,18 +1774,18 @@
         <v>1.34</v>
       </c>
       <c r="D23" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E23">
         <v>180</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>1.91</v>
@@ -1794,18 +1794,18 @@
         <v>1.52</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E24">
         <v>270</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>2.23</v>
@@ -1814,18 +1814,18 @@
         <v>1.68</v>
       </c>
       <c r="D25" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E25">
         <v>180</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>2.14</v>
@@ -1834,18 +1834,18 @@
         <v>1.73</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E26">
         <v>180</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <v>2.2850000000000001</v>
@@ -1854,18 +1854,18 @@
         <v>1.575</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E27">
         <v>180</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>1.97</v>
@@ -1874,18 +1874,18 @@
         <v>1.43</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E28">
         <v>90</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>2.0249999999999999</v>
@@ -1894,18 +1894,18 @@
         <v>1.44</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E29">
         <v>90</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30">
         <v>2.17</v>
@@ -1914,18 +1914,18 @@
         <v>1.43</v>
       </c>
       <c r="D30" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E30">
         <v>90</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>2.1150000000000002</v>
@@ -1934,18 +1934,18 @@
         <v>1.44</v>
       </c>
       <c r="D31" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E31">
         <v>90</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>0.56999999999999995</v>
@@ -1954,18 +1954,18 @@
         <v>1.8</v>
       </c>
       <c r="D32" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E32">
         <v>270</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>0.9</v>
@@ -1974,18 +1974,18 @@
         <v>1.75</v>
       </c>
       <c r="D33" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E33">
         <v>180</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>1.2250000000000001</v>
@@ -1994,18 +1994,18 @@
         <v>1.7250000000000001</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>1.06</v>
@@ -2014,18 +2014,18 @@
         <v>1.5</v>
       </c>
       <c r="D35" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E35">
         <v>270</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36">
         <v>0.31</v>
@@ -2034,18 +2034,18 @@
         <v>0.2</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E36">
         <v>270</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37">
         <v>2.13</v>
@@ -2054,18 +2054,18 @@
         <v>0.76500000000000001</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38">
         <v>2.105</v>
@@ -2074,18 +2074,18 @@
         <v>1.3</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E38">
         <v>90</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39">
         <v>2.06</v>
@@ -2094,18 +2094,18 @@
         <v>0.36</v>
       </c>
       <c r="D39" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E39">
         <v>270</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40">
         <v>2.7050000000000001</v>
@@ -2114,18 +2114,18 @@
         <v>0.25</v>
       </c>
       <c r="D40" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E40">
         <v>270</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41">
         <v>2.605</v>
@@ -2134,18 +2134,18 @@
         <v>0.25</v>
       </c>
       <c r="D41" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E41">
         <v>270</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42">
         <v>2.5049999999999999</v>
@@ -2154,18 +2154,18 @@
         <v>0.25</v>
       </c>
       <c r="D42" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E42">
         <v>270</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>2.4049999999999998</v>
@@ -2174,18 +2174,18 @@
         <v>0.25</v>
       </c>
       <c r="D43" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E43">
         <v>270</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>2.3050000000000002</v>
@@ -2194,18 +2194,18 @@
         <v>0.25</v>
       </c>
       <c r="D44" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E44">
         <v>270</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <v>2.2050000000000001</v>
@@ -2214,18 +2214,18 @@
         <v>0.25</v>
       </c>
       <c r="D45" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E45">
         <v>270</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <v>0.59</v>
@@ -2234,18 +2234,18 @@
         <v>1.38</v>
       </c>
       <c r="D46" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>0.69499999999999995</v>
@@ -2254,18 +2254,18 @@
         <v>1.02</v>
       </c>
       <c r="D47" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E47">
         <v>90</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48">
         <v>2.42</v>
@@ -2274,18 +2274,18 @@
         <v>0.77</v>
       </c>
       <c r="D48" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E48">
         <v>270</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>0.78</v>
@@ -2294,18 +2294,18 @@
         <v>0.67500000000000004</v>
       </c>
       <c r="D49" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E49">
         <v>180</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>0.105</v>
@@ -2314,18 +2314,18 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="D50" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51">
         <v>0.105</v>
@@ -2334,18 +2334,18 @@
         <v>0.1</v>
       </c>
       <c r="D51" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52">
         <v>2.5449999999999999</v>
@@ -2354,18 +2354,18 @@
         <v>1.655</v>
       </c>
       <c r="D52" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E52">
         <v>270</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>2.4249999999999998</v>
@@ -2374,18 +2374,18 @@
         <v>1.575</v>
       </c>
       <c r="D53" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E53">
         <v>180</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>1.92</v>
@@ -2394,18 +2394,18 @@
         <v>1.595</v>
       </c>
       <c r="D54" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E54">
         <v>180</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>1.6</v>
@@ -2414,18 +2414,18 @@
         <v>0.52</v>
       </c>
       <c r="D55" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56">
         <v>2.3050000000000002</v>
@@ -2434,18 +2434,18 @@
         <v>1.65</v>
       </c>
       <c r="D56" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E56">
         <v>90</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57">
         <v>2.21</v>
@@ -2454,18 +2454,18 @@
         <v>1.5449999999999999</v>
       </c>
       <c r="D57" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E57">
         <v>90</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58">
         <v>0.78500000000000003</v>
@@ -2474,18 +2474,18 @@
         <v>1.4850000000000001</v>
       </c>
       <c r="D58" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B59">
         <v>0.69</v>
@@ -2494,18 +2494,18 @@
         <v>1.9950000000000001</v>
       </c>
       <c r="D59" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E59">
         <v>180</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60">
         <v>0.12</v>
@@ -2514,18 +2514,18 @@
         <v>1.125</v>
       </c>
       <c r="D60" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E60">
         <v>180</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B61">
         <v>0.45500000000000002</v>
@@ -2534,18 +2534,18 @@
         <v>1.64</v>
       </c>
       <c r="D61" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62">
         <v>0.40500000000000003</v>
@@ -2554,18 +2554,18 @@
         <v>1.355</v>
       </c>
       <c r="D62" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E62">
         <v>180</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63">
         <v>0.20499999999999999</v>
@@ -2574,18 +2574,18 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="D63" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E63">
         <v>180</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B64">
         <v>0.20499999999999999</v>
@@ -2594,18 +2594,18 @@
         <v>0.1</v>
       </c>
       <c r="D64" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E64">
         <v>180</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B65">
         <v>1.49</v>
@@ -2614,18 +2614,18 @@
         <v>0.65500000000000003</v>
       </c>
       <c r="D65" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E65">
         <v>180</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B66">
         <v>1.405</v>
@@ -2634,18 +2634,18 @@
         <v>0.43</v>
       </c>
       <c r="D66" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E66">
         <v>180</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B67">
         <v>2.0699999999999998</v>
@@ -2654,18 +2654,18 @@
         <v>1.45</v>
       </c>
       <c r="D67" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E67">
         <v>270</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68">
         <v>0.52500000000000002</v>
@@ -2674,18 +2674,18 @@
         <v>1.81</v>
       </c>
       <c r="D68" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E68">
         <v>90</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B69">
         <v>0.435</v>
@@ -2694,18 +2694,18 @@
         <v>1.5449999999999999</v>
       </c>
       <c r="D69" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E69">
         <v>180</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B70">
         <v>0.22500000000000001</v>
@@ -2714,18 +2714,18 @@
         <v>1.085</v>
       </c>
       <c r="D70" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B71">
         <v>0.59</v>
@@ -2734,18 +2734,18 @@
         <v>0.89500000000000002</v>
       </c>
       <c r="D71" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E71">
         <v>180</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B72">
         <v>0.59</v>
@@ -2754,18 +2754,18 @@
         <v>0.94</v>
       </c>
       <c r="D72" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73">
         <v>2.3199999999999998</v>
@@ -2774,18 +2774,18 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="D73" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E73">
         <v>90</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B74">
         <v>2.0499999999999998</v>
@@ -2794,18 +2794,18 @@
         <v>0.255</v>
       </c>
       <c r="D74" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E74">
         <v>270</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B75">
         <v>2.0049999999999999</v>
@@ -2814,18 +2814,18 @@
         <v>0.255</v>
       </c>
       <c r="D75" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E75">
         <v>90</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B76">
         <v>2.0049999999999999</v>
@@ -2834,18 +2834,18 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="D76" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E76">
         <v>90</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B77">
         <v>2.6549999999999998</v>
@@ -2854,18 +2854,18 @@
         <v>0.27</v>
       </c>
       <c r="D77" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E77">
         <v>90</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B78">
         <v>2.5550000000000002</v>
@@ -2874,18 +2874,18 @@
         <v>0.27</v>
       </c>
       <c r="D78" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E78">
         <v>90</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B79">
         <v>2.4550000000000001</v>
@@ -2894,18 +2894,18 @@
         <v>0.27</v>
       </c>
       <c r="D79" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E79">
         <v>90</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B80">
         <v>2.2549999999999999</v>
@@ -2914,18 +2914,18 @@
         <v>0.27</v>
       </c>
       <c r="D80" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E80">
         <v>90</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B81">
         <v>2.1549999999999998</v>
@@ -2934,18 +2934,18 @@
         <v>0.27</v>
       </c>
       <c r="D81" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E81">
         <v>90</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B82">
         <v>1.865</v>
@@ -2954,18 +2954,18 @@
         <v>0.76500000000000001</v>
       </c>
       <c r="D82" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E82">
         <v>180</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B83">
         <v>0.32</v>
@@ -2974,18 +2974,18 @@
         <v>1.5649999999999999</v>
       </c>
       <c r="D83" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E83">
         <v>90</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B84">
         <v>0.61</v>
@@ -2994,18 +2994,18 @@
         <v>1.05</v>
       </c>
       <c r="D84" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E84">
         <v>270</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B85">
         <v>2.0750000000000002</v>
@@ -3014,18 +3014,18 @@
         <v>1.6</v>
       </c>
       <c r="D85" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E85">
         <v>180</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B86">
         <v>1.7949999999999999</v>
@@ -3034,18 +3034,18 @@
         <v>1.595</v>
       </c>
       <c r="D86" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E86">
         <v>180</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B87">
         <v>1.075</v>
@@ -3054,18 +3054,18 @@
         <v>1.65</v>
       </c>
       <c r="D87" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E87">
         <v>270</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B88">
         <v>0.245</v>
@@ -3074,18 +3074,18 @@
         <v>0.48499999999999999</v>
       </c>
       <c r="D88" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E88">
         <v>90</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B89">
         <v>1.99</v>
@@ -3094,18 +3094,18 @@
         <v>1.19</v>
       </c>
       <c r="D89" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B90">
         <v>2.3450000000000002</v>
@@ -3114,18 +3114,18 @@
         <v>0.97</v>
       </c>
       <c r="D90" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E90">
         <v>270</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B91">
         <v>0.73499999999999999</v>
@@ -3134,18 +3134,18 @@
         <v>1.74</v>
       </c>
       <c r="D91" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E91">
         <v>90</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B92">
         <v>0.58499999999999996</v>
@@ -3154,18 +3154,18 @@
         <v>1.62</v>
       </c>
       <c r="D92" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E92">
         <v>90</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B93">
         <v>1.585</v>
@@ -3174,18 +3174,18 @@
         <v>0.76500000000000001</v>
       </c>
       <c r="D93" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E93">
         <v>90</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B94">
         <v>1.7250000000000001</v>
@@ -3194,18 +3194,18 @@
         <v>0.38</v>
       </c>
       <c r="D94" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E94">
         <v>180</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B95">
         <v>1.55</v>
@@ -3214,18 +3214,18 @@
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E95">
         <v>270</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B96">
         <v>0.63</v>
@@ -3234,18 +3234,18 @@
         <v>1.76</v>
       </c>
       <c r="D96" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E96">
         <v>270</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B97">
         <v>0.89</v>
@@ -3254,18 +3254,18 @@
         <v>1.8149999999999999</v>
       </c>
       <c r="D97" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B98">
         <v>1.1000000000000001</v>
@@ -3274,13 +3274,13 @@
         <v>0.97499999999999998</v>
       </c>
       <c r="D98" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="E98">
         <v>270</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed mousebites and re-exported gerbers as well as drill files. Also realizes I didn't have the INSERT set for fiducials so I set that an exported XY position/rotation data for fiducials.
</commit_message>
<xml_diff>
--- a/Kicad-Faraday/OutputFiles/Faraday-all.xlsx
+++ b/Kicad-Faraday/OutputFiles/Faraday-all.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="158">
   <si>
     <t>Side</t>
   </si>
@@ -472,6 +472,27 @@
   </si>
   <si>
     <t>Bottom</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FIDUCIAL</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>FD3</t>
+  </si>
+  <si>
+    <t>FD4</t>
+  </si>
+  <si>
+    <t>FD5</t>
+  </si>
+  <si>
+    <t>FD6</t>
   </si>
 </sst>
 </file>
@@ -1315,13 +1336,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="6" max="6" width="9.06640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -3283,6 +3307,126 @@
         <v>8</v>
       </c>
     </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>151</v>
+      </c>
+      <c r="B99">
+        <v>2.86</v>
+      </c>
+      <c r="C99">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D99" t="s">
+        <v>149</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>153</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100" t="s">
+        <v>149</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>154</v>
+      </c>
+      <c r="B101">
+        <v>2.86</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101" t="s">
+        <v>149</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>155</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102" t="s">
+        <v>150</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>156</v>
+      </c>
+      <c r="B103">
+        <v>2.84</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103" t="s">
+        <v>150</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>157</v>
+      </c>
+      <c r="B104">
+        <v>2.84</v>
+      </c>
+      <c r="C104">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D104" t="s">
+        <v>150</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated pick and place files to work with PCB:NG better. Also exported gerbers and drill files relative to aux axis for PCB:NG.
</commit_message>
<xml_diff>
--- a/Kicad-Faraday/OutputFiles/Faraday-all.xlsx
+++ b/Kicad-Faraday/OutputFiles/Faraday-all.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="140">
   <si>
     <t>Side</t>
   </si>
@@ -42,15 +42,6 @@
     <t>C6</t>
   </si>
   <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>DNP</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
     <t>C9</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>C21</t>
   </si>
   <si>
-    <t>C22</t>
-  </si>
-  <si>
     <t>C23</t>
   </si>
   <si>
@@ -150,9 +138,6 @@
     <t>C50</t>
   </si>
   <si>
-    <t>C51</t>
-  </si>
-  <si>
     <t>C52</t>
   </si>
   <si>
@@ -165,9 +150,6 @@
     <t>C56</t>
   </si>
   <si>
-    <t>C57</t>
-  </si>
-  <si>
     <t>C63</t>
   </si>
   <si>
@@ -252,9 +234,6 @@
     <t>R15</t>
   </si>
   <si>
-    <t>R18</t>
-  </si>
-  <si>
     <t>R20</t>
   </si>
   <si>
@@ -318,9 +297,6 @@
     <t>23K256T-I/ST</t>
   </si>
   <si>
-    <t>U9</t>
-  </si>
-  <si>
     <t>U10</t>
   </si>
   <si>
@@ -351,18 +327,9 @@
     <t>Z2</t>
   </si>
   <si>
-    <t>P2</t>
-  </si>
-  <si>
     <t>RefDes</t>
   </si>
   <si>
-    <t>X (mil)</t>
-  </si>
-  <si>
-    <t>Y (mil)</t>
-  </si>
-  <si>
     <t>Rotate</t>
   </si>
   <si>
@@ -456,9 +423,6 @@
     <t>MIC94072YC6-TR</t>
   </si>
   <si>
-    <t>IS25LQ080-JNLE-TR</t>
-  </si>
-  <si>
     <t>LTC4412ES6#TRMPBF</t>
   </si>
   <si>
@@ -471,28 +435,10 @@
     <t>Top</t>
   </si>
   <si>
-    <t>Bottom</t>
-  </si>
-  <si>
-    <t>FD1</t>
-  </si>
-  <si>
-    <t>FIDUCIAL</t>
-  </si>
-  <si>
-    <t>FD2</t>
-  </si>
-  <si>
-    <t>FD3</t>
-  </si>
-  <si>
-    <t>FD4</t>
-  </si>
-  <si>
-    <t>FD5</t>
-  </si>
-  <si>
-    <t>FD6</t>
+    <t>X (in)</t>
+  </si>
+  <si>
+    <t>Y (in)</t>
   </si>
 </sst>
 </file>
@@ -1336,35 +1282,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84:F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="6" width="9.06640625" customWidth="1"/>
+    <col min="6" max="6" width="24.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -1378,13 +1324,13 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E2">
         <v>270</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1398,13 +1344,13 @@
         <v>0.51</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E3">
         <v>270</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -1418,13 +1364,13 @@
         <v>0.875</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -1438,13 +1384,13 @@
         <v>0.82</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -1458,13 +1404,13 @@
         <v>1.03</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E6">
         <v>90</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -1478,13 +1424,13 @@
         <v>1.02</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E7">
         <v>90</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -1492,859 +1438,859 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1.83</v>
+        <v>1.5649999999999999</v>
       </c>
       <c r="C8">
-        <v>0.39</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E8">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>1.62</v>
+        <v>0.59</v>
       </c>
       <c r="C9">
-        <v>0.39</v>
+        <v>1.26</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E9">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>1.5649999999999999</v>
+        <v>1.5349999999999999</v>
       </c>
       <c r="C10">
-        <v>1.0900000000000001</v>
+        <v>0.91</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E10">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>0.59</v>
+        <v>1.85</v>
       </c>
       <c r="C11">
-        <v>1.26</v>
+        <v>0.505</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>1.5349999999999999</v>
+        <v>1.5</v>
       </c>
       <c r="C12">
-        <v>0.91</v>
+        <v>0.61</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>1.85</v>
+        <v>1.575</v>
       </c>
       <c r="C13">
-        <v>0.505</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E13">
         <v>270</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>1.5</v>
+        <v>0.16</v>
       </c>
       <c r="C14">
-        <v>0.61</v>
+        <v>0.23</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E14">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>1.575</v>
+        <v>1.5</v>
       </c>
       <c r="C15">
-        <v>0.59499999999999997</v>
+        <v>0.52</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E15">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>0.16</v>
+        <v>2.5</v>
       </c>
       <c r="C16">
-        <v>0.23</v>
+        <v>1.605</v>
       </c>
       <c r="D16" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>1.5</v>
       </c>
       <c r="C17">
-        <v>0.52</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="D17" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E17">
         <v>180</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>2.5</v>
+        <v>2.355</v>
       </c>
       <c r="C18">
         <v>1.605</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E18">
         <v>90</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>1.5</v>
+        <v>1.405</v>
       </c>
       <c r="C19">
-        <v>0.56499999999999995</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="D19" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E19">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>2.355</v>
+        <v>0.8</v>
       </c>
       <c r="C20">
-        <v>1.605</v>
+        <v>1.34</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E20">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>1.405</v>
+        <v>1.91</v>
       </c>
       <c r="C21">
-        <v>0.47499999999999998</v>
+        <v>1.52</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>0.61</v>
+        <v>2.23</v>
       </c>
       <c r="C22">
-        <v>1.18</v>
+        <v>1.68</v>
       </c>
       <c r="D22" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>0.8</v>
+        <v>2.14</v>
       </c>
       <c r="C23">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E23">
         <v>180</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>1.91</v>
+        <v>2.2850000000000001</v>
       </c>
       <c r="C24">
-        <v>1.52</v>
+        <v>1.575</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E24">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>2.23</v>
+        <v>1.97</v>
       </c>
       <c r="C25">
-        <v>1.68</v>
+        <v>1.43</v>
       </c>
       <c r="D25" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E25">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>2.14</v>
+        <v>2.0249999999999999</v>
       </c>
       <c r="C26">
-        <v>1.73</v>
+        <v>1.44</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E26">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>2.2850000000000001</v>
+        <v>2.17</v>
       </c>
       <c r="C27">
-        <v>1.575</v>
+        <v>1.43</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E27">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>1.97</v>
+        <v>2.1150000000000002</v>
       </c>
       <c r="C28">
-        <v>1.43</v>
+        <v>1.44</v>
       </c>
       <c r="D28" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E28">
         <v>90</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>2.0249999999999999</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C29">
-        <v>1.44</v>
+        <v>1.8</v>
       </c>
       <c r="D29" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E29">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
-        <v>2.17</v>
+        <v>0.9</v>
       </c>
       <c r="C30">
-        <v>1.43</v>
+        <v>1.75</v>
       </c>
       <c r="D30" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E30">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
-        <v>2.1150000000000002</v>
+        <v>1.2250000000000001</v>
       </c>
       <c r="C31">
-        <v>1.44</v>
+        <v>1.7250000000000001</v>
       </c>
       <c r="D31" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E31">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32">
-        <v>0.56999999999999995</v>
+        <v>1.06</v>
       </c>
       <c r="C32">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="D32" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E32">
         <v>270</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33">
-        <v>0.9</v>
+        <v>0.31</v>
       </c>
       <c r="C33">
-        <v>1.75</v>
+        <v>0.2</v>
       </c>
       <c r="D33" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E33">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34">
-        <v>1.2250000000000001</v>
+        <v>2.13</v>
       </c>
       <c r="C34">
-        <v>1.7250000000000001</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="D34" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
-        <v>1.06</v>
+        <v>2.105</v>
       </c>
       <c r="C35">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="D35" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E35">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36">
-        <v>0.31</v>
+        <v>2.06</v>
       </c>
       <c r="C36">
-        <v>0.2</v>
+        <v>0.36</v>
       </c>
       <c r="D36" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E36">
         <v>270</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
-        <v>2.13</v>
+        <v>2.7050000000000001</v>
       </c>
       <c r="C37">
-        <v>0.76500000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="D37" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38">
-        <v>2.105</v>
+        <v>2.605</v>
       </c>
       <c r="C38">
-        <v>1.3</v>
+        <v>0.25</v>
       </c>
       <c r="D38" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E38">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39">
-        <v>2.06</v>
+        <v>2.5049999999999999</v>
       </c>
       <c r="C39">
-        <v>0.36</v>
+        <v>0.25</v>
       </c>
       <c r="D39" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E39">
         <v>270</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40">
-        <v>2.7050000000000001</v>
+        <v>2.3050000000000002</v>
       </c>
       <c r="C40">
         <v>0.25</v>
       </c>
       <c r="D40" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E40">
         <v>270</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41">
-        <v>2.605</v>
+        <v>2.2050000000000001</v>
       </c>
       <c r="C41">
         <v>0.25</v>
       </c>
       <c r="D41" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E41">
         <v>270</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42">
-        <v>2.5049999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="C42">
-        <v>0.25</v>
+        <v>1.38</v>
       </c>
       <c r="D42" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E42">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43">
-        <v>2.4049999999999998</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="C43">
-        <v>0.25</v>
+        <v>1.02</v>
       </c>
       <c r="D43" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E43">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44">
-        <v>2.3050000000000002</v>
+        <v>0.78</v>
       </c>
       <c r="C44">
-        <v>0.25</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="D44" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E44">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45">
-        <v>2.2050000000000001</v>
+        <v>0.105</v>
       </c>
       <c r="C45">
-        <v>0.25</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E45">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46">
-        <v>0.59</v>
+        <v>0.105</v>
       </c>
       <c r="C46">
-        <v>1.38</v>
+        <v>0.1</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47">
-        <v>0.69499999999999995</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="C47">
-        <v>1.02</v>
+        <v>1.655</v>
       </c>
       <c r="D47" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E47">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48">
-        <v>2.42</v>
+        <v>2.4249999999999998</v>
       </c>
       <c r="C48">
-        <v>0.77</v>
+        <v>1.575</v>
       </c>
       <c r="D48" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E48">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>8</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49">
-        <v>0.78</v>
+        <v>1.92</v>
       </c>
       <c r="C49">
-        <v>0.67500000000000004</v>
+        <v>1.595</v>
       </c>
       <c r="D49" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E49">
         <v>180</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50">
-        <v>0.105</v>
+        <v>1.6</v>
       </c>
       <c r="C50">
-        <v>4.4999999999999998E-2</v>
+        <v>0.52</v>
       </c>
       <c r="D50" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>128</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
@@ -2352,19 +2298,19 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>0.105</v>
+        <v>2.3050000000000002</v>
       </c>
       <c r="C51">
-        <v>0.1</v>
+        <v>1.65</v>
       </c>
       <c r="D51" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
@@ -2372,19 +2318,19 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>2.5449999999999999</v>
+        <v>2.21</v>
       </c>
       <c r="C52">
-        <v>1.655</v>
+        <v>1.5449999999999999</v>
       </c>
       <c r="D52" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E52">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
@@ -2392,19 +2338,19 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>2.4249999999999998</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="C53">
-        <v>1.575</v>
+        <v>1.4850000000000001</v>
       </c>
       <c r="D53" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E53">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
@@ -2412,139 +2358,139 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>1.92</v>
+        <v>0.69</v>
       </c>
       <c r="C54">
-        <v>1.595</v>
+        <v>1.9950000000000001</v>
       </c>
       <c r="D54" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E54">
         <v>180</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B55">
-        <v>1.6</v>
+        <v>0.12</v>
       </c>
       <c r="C55">
-        <v>0.52</v>
+        <v>1.125</v>
       </c>
       <c r="D55" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B56">
-        <v>2.3050000000000002</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="C56">
-        <v>1.65</v>
+        <v>1.64</v>
       </c>
       <c r="D56" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E56">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>131</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B57">
-        <v>2.21</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="C57">
-        <v>1.5449999999999999</v>
+        <v>1.355</v>
       </c>
       <c r="D57" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E57">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B58">
-        <v>0.78500000000000003</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="C58">
-        <v>1.4850000000000001</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D58" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B59">
-        <v>0.69</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="C59">
-        <v>1.9950000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D59" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E59">
         <v>180</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B60">
-        <v>0.12</v>
+        <v>1.49</v>
       </c>
       <c r="C60">
-        <v>1.125</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="D60" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E60">
         <v>180</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
@@ -2552,359 +2498,359 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>0.45500000000000002</v>
+        <v>1.405</v>
       </c>
       <c r="C61">
-        <v>1.64</v>
+        <v>0.43</v>
       </c>
       <c r="D61" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62">
-        <v>0.40500000000000003</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="C62">
-        <v>1.355</v>
+        <v>1.45</v>
       </c>
       <c r="D62" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E62">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63">
-        <v>0.20499999999999999</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="C63">
-        <v>4.4999999999999998E-2</v>
+        <v>1.81</v>
       </c>
       <c r="D63" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E63">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64">
-        <v>0.20499999999999999</v>
+        <v>0.435</v>
       </c>
       <c r="C64">
-        <v>0.1</v>
+        <v>1.5449999999999999</v>
       </c>
       <c r="D64" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E64">
         <v>180</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65">
-        <v>1.49</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="C65">
-        <v>0.65500000000000003</v>
+        <v>1.085</v>
       </c>
       <c r="D65" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E65">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66">
-        <v>1.405</v>
+        <v>0.59</v>
       </c>
       <c r="C66">
-        <v>0.43</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="D66" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E66">
         <v>180</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67">
-        <v>2.0699999999999998</v>
+        <v>0.59</v>
       </c>
       <c r="C67">
-        <v>1.45</v>
+        <v>0.94</v>
       </c>
       <c r="D67" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E67">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68">
-        <v>0.52500000000000002</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="C68">
-        <v>1.81</v>
+        <v>0.255</v>
       </c>
       <c r="D68" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E68">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69">
-        <v>0.435</v>
+        <v>2.0049999999999999</v>
       </c>
       <c r="C69">
-        <v>1.5449999999999999</v>
+        <v>0.255</v>
       </c>
       <c r="D69" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E69">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70">
-        <v>0.22500000000000001</v>
+        <v>2.0049999999999999</v>
       </c>
       <c r="C70">
-        <v>1.085</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="D70" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71">
-        <v>0.59</v>
+        <v>2.6549999999999998</v>
       </c>
       <c r="C71">
-        <v>0.89500000000000002</v>
+        <v>0.27</v>
       </c>
       <c r="D71" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E71">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B72">
-        <v>0.59</v>
+        <v>2.5550000000000002</v>
       </c>
       <c r="C72">
-        <v>0.94</v>
+        <v>0.27</v>
       </c>
       <c r="D72" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73">
-        <v>2.3199999999999998</v>
+        <v>2.4550000000000001</v>
       </c>
       <c r="C73">
-        <v>1.1599999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="D73" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E73">
         <v>90</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B74">
-        <v>2.0499999999999998</v>
+        <v>2.2549999999999999</v>
       </c>
       <c r="C74">
-        <v>0.255</v>
+        <v>0.27</v>
       </c>
       <c r="D74" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E74">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B75">
-        <v>2.0049999999999999</v>
+        <v>2.1549999999999998</v>
       </c>
       <c r="C75">
-        <v>0.255</v>
+        <v>0.27</v>
       </c>
       <c r="D75" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E75">
         <v>90</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B76">
-        <v>2.0049999999999999</v>
+        <v>1.865</v>
       </c>
       <c r="C76">
-        <v>0.34499999999999997</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="D76" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E76">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B77">
-        <v>2.6549999999999998</v>
+        <v>0.32</v>
       </c>
       <c r="C77">
-        <v>0.27</v>
+        <v>1.5649999999999999</v>
       </c>
       <c r="D77" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E77">
         <v>90</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78">
+        <v>0.61</v>
+      </c>
+      <c r="C78">
+        <v>1.05</v>
+      </c>
+      <c r="D78" t="s">
+        <v>137</v>
+      </c>
+      <c r="E78">
+        <v>270</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B78">
-        <v>2.5550000000000002</v>
-      </c>
-      <c r="C78">
-        <v>0.27</v>
-      </c>
-      <c r="D78" t="s">
-        <v>149</v>
-      </c>
-      <c r="E78">
-        <v>90</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
@@ -2912,19 +2858,19 @@
         <v>83</v>
       </c>
       <c r="B79">
-        <v>2.4550000000000001</v>
+        <v>2.0750000000000002</v>
       </c>
       <c r="C79">
-        <v>0.27</v>
+        <v>1.6</v>
       </c>
       <c r="D79" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E79">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
@@ -2932,499 +2878,219 @@
         <v>84</v>
       </c>
       <c r="B80">
-        <v>2.2549999999999999</v>
+        <v>1.7949999999999999</v>
       </c>
       <c r="C80">
-        <v>0.27</v>
+        <v>1.595</v>
       </c>
       <c r="D80" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E80">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B81">
-        <v>2.1549999999999998</v>
+        <v>1.075</v>
       </c>
       <c r="C81">
-        <v>0.27</v>
+        <v>1.65</v>
       </c>
       <c r="D81" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E81">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B82">
-        <v>1.865</v>
+        <v>0.245</v>
       </c>
       <c r="C82">
-        <v>0.76500000000000001</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="D82" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E82">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B83">
-        <v>0.32</v>
+        <v>1.99</v>
       </c>
       <c r="C83">
-        <v>1.5649999999999999</v>
+        <v>1.19</v>
       </c>
       <c r="D83" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E83">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B84">
-        <v>0.61</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="C84">
-        <v>1.05</v>
+        <v>1.74</v>
       </c>
       <c r="D84" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E84">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="C85">
+        <v>1.62</v>
+      </c>
+      <c r="D85" t="s">
+        <v>137</v>
+      </c>
+      <c r="E85">
         <v>90</v>
       </c>
-      <c r="B85">
-        <v>2.0750000000000002</v>
-      </c>
-      <c r="C85">
-        <v>1.6</v>
-      </c>
-      <c r="D85" t="s">
-        <v>149</v>
-      </c>
-      <c r="E85">
-        <v>180</v>
-      </c>
       <c r="F85" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B86">
-        <v>1.7949999999999999</v>
+        <v>1.585</v>
       </c>
       <c r="C86">
-        <v>1.595</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="D86" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E86">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B87">
-        <v>1.075</v>
+        <v>1.7250000000000001</v>
       </c>
       <c r="C87">
-        <v>1.65</v>
+        <v>0.38</v>
       </c>
       <c r="D87" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E87">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>94</v>
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B88">
-        <v>0.245</v>
+        <v>1.55</v>
       </c>
       <c r="C88">
-        <v>0.48499999999999999</v>
+        <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E88">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B89">
-        <v>1.99</v>
+        <v>0.63</v>
       </c>
       <c r="C89">
-        <v>1.19</v>
+        <v>1.76</v>
       </c>
       <c r="D89" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B90">
-        <v>2.3450000000000002</v>
+        <v>0.89</v>
       </c>
       <c r="C90">
-        <v>0.97</v>
+        <v>1.8149999999999999</v>
       </c>
       <c r="D90" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E90">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A91" t="s">
         <v>100</v>
-      </c>
-      <c r="B91">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="C91">
-        <v>1.74</v>
-      </c>
-      <c r="D91" t="s">
-        <v>149</v>
-      </c>
-      <c r="E91">
-        <v>90</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A92" t="s">
-        <v>102</v>
-      </c>
-      <c r="B92">
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="C92">
-        <v>1.62</v>
-      </c>
-      <c r="D92" t="s">
-        <v>149</v>
-      </c>
-      <c r="E92">
-        <v>90</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A93" t="s">
-        <v>103</v>
-      </c>
-      <c r="B93">
-        <v>1.585</v>
-      </c>
-      <c r="C93">
-        <v>0.76500000000000001</v>
-      </c>
-      <c r="D93" t="s">
-        <v>149</v>
-      </c>
-      <c r="E93">
-        <v>90</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A94" t="s">
-        <v>105</v>
-      </c>
-      <c r="B94">
-        <v>1.7250000000000001</v>
-      </c>
-      <c r="C94">
-        <v>0.38</v>
-      </c>
-      <c r="D94" t="s">
-        <v>149</v>
-      </c>
-      <c r="E94">
-        <v>180</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A95" t="s">
-        <v>106</v>
-      </c>
-      <c r="B95">
-        <v>1.55</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-      <c r="D95" t="s">
-        <v>149</v>
-      </c>
-      <c r="E95">
-        <v>270</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A96" t="s">
-        <v>107</v>
-      </c>
-      <c r="B96">
-        <v>0.63</v>
-      </c>
-      <c r="C96">
-        <v>1.76</v>
-      </c>
-      <c r="D96" t="s">
-        <v>149</v>
-      </c>
-      <c r="E96">
-        <v>270</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A97" t="s">
-        <v>109</v>
-      </c>
-      <c r="B97">
-        <v>0.89</v>
-      </c>
-      <c r="C97">
-        <v>1.8149999999999999</v>
-      </c>
-      <c r="D97" t="s">
-        <v>149</v>
-      </c>
-      <c r="E97">
-        <v>0</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A98" t="s">
-        <v>110</v>
-      </c>
-      <c r="B98">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C98">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="D98" t="s">
-        <v>150</v>
-      </c>
-      <c r="E98">
-        <v>270</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A99" t="s">
-        <v>151</v>
-      </c>
-      <c r="B99">
-        <v>2.86</v>
-      </c>
-      <c r="C99">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="D99" t="s">
-        <v>149</v>
-      </c>
-      <c r="E99">
-        <v>0</v>
-      </c>
-      <c r="F99" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A100" t="s">
-        <v>153</v>
-      </c>
-      <c r="B100">
-        <v>0</v>
-      </c>
-      <c r="C100">
-        <v>0</v>
-      </c>
-      <c r="D100" t="s">
-        <v>149</v>
-      </c>
-      <c r="E100">
-        <v>0</v>
-      </c>
-      <c r="F100" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
-        <v>154</v>
-      </c>
-      <c r="B101">
-        <v>2.86</v>
-      </c>
-      <c r="C101">
-        <v>0</v>
-      </c>
-      <c r="D101" t="s">
-        <v>149</v>
-      </c>
-      <c r="E101">
-        <v>0</v>
-      </c>
-      <c r="F101" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A102" t="s">
-        <v>155</v>
-      </c>
-      <c r="B102">
-        <v>0</v>
-      </c>
-      <c r="C102">
-        <v>0</v>
-      </c>
-      <c r="D102" t="s">
-        <v>150</v>
-      </c>
-      <c r="E102">
-        <v>0</v>
-      </c>
-      <c r="F102" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A103" t="s">
-        <v>156</v>
-      </c>
-      <c r="B103">
-        <v>2.84</v>
-      </c>
-      <c r="C103">
-        <v>0</v>
-      </c>
-      <c r="D103" t="s">
-        <v>150</v>
-      </c>
-      <c r="E103">
-        <v>0</v>
-      </c>
-      <c r="F103" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A104" t="s">
-        <v>157</v>
-      </c>
-      <c r="B104">
-        <v>2.84</v>
-      </c>
-      <c r="C104">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="D104" t="s">
-        <v>150</v>
-      </c>
-      <c r="E104">
-        <v>0</v>
-      </c>
-      <c r="F104" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>